<commit_message>
Added 9 and 10
</commit_message>
<xml_diff>
--- a/project1/MasterExperiment.xlsx
+++ b/project1/MasterExperiment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="400" windowWidth="50560" windowHeight="24840" tabRatio="500"/>
+    <workbookView xWindow="380" yWindow="100" windowWidth="50560" windowHeight="26280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MasterExperiment.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="84">
   <si>
     <t>Your</t>
   </si>
@@ -236,6 +236,42 @@
   <si>
     <t>There is a pattern formed of triangles of different sizes in chaotic manner as well but patterns are very small.</t>
   </si>
+  <si>
+    <t>This picture is somewhere in between class 3 and 4. It is very complex but has "holes" of homogeneous structures in the whole picture. Triangle structures don't look like the ones spicific for class 3 too.</t>
+  </si>
+  <si>
+    <t>This picture is very similar to one before but it's vay more apperiodic. It is closer to class 3</t>
+  </si>
+  <si>
+    <t>Same and even smaller patterns</t>
+  </si>
+  <si>
+    <t>This is an interesting pattern. There diagonal lines forming triangle-like structures, there is a lot of class 2 forms on this picture along with chaos from class 3.</t>
+  </si>
+  <si>
+    <t>This structure is very chaotic. And even though there are some kind of periodic line in there, they are very small, and also tend to be in random order.</t>
+  </si>
+  <si>
+    <t>Very long transient period with random triangle-like structures along its length</t>
+  </si>
+  <si>
+    <t>There is a short transient period, and then each cell turns into the same state, pink(0) or blue(1) - lines, and never changes.</t>
+  </si>
+  <si>
+    <t>Very chaotic pattern , it's also very complex. There is something from class 4, but it better fits for class 3</t>
+  </si>
+  <si>
+    <t>Very aperiodic pattern</t>
+  </si>
+  <si>
+    <t>There is a long pretty transient period, and then cell turns into the same state, blue(1), and never changes.</t>
+  </si>
+  <si>
+    <t>There is short transient period here, but we have 3 line-like periodic formations.They are the same as well.</t>
+  </si>
+  <si>
+    <t>Same but they are also yellow lines along with pink background. Cells still transform into homogeneous state endlessly</t>
+  </si>
 </sst>
 </file>
 
@@ -336,8 +372,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -443,7 +497,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="99">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -484,6 +538,15 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -524,12 +587,25 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFEF08"/>
+      <color rgb="FFC5090D"/>
+      <color rgb="FF19FF37"/>
+      <color rgb="FF07F3FF"/>
       <color rgb="FFD976D0"/>
     </mruColors>
   </colors>
@@ -1027,6 +1103,806 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Experiment 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$D$84:$D$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.848</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.824</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.688</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.608</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.455999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.408</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.288</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.144</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$84:$J$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Experiment 5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="660066"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$D$102:$D$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.912</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.792</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.671999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.663999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.616</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.592</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.439999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.296</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.248</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.223999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$102:$J$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Experiment 6</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$D$120:$D$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.912</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.904</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.592</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.512</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.488</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.344</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.223999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$120:$J$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Experiment 7</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="19FF37"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$D$138:$D$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.968</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.888</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.744</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.552</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.504</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.424</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.272</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.248</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.128</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.008</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$138:$J$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>Experiment 8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="C5090D"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$D$156:$D$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.944</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.824</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.679999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.455999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.408</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.352</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$156:$J$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Experiment 9</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="07F3FF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$D$174:$D$186</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.912</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.888</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.688</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.544</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.424</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.304</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.296</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.128</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$174:$J$186</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:v>Experiment 10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FFEF08"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$D$192:$D$204</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.848</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.728</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.679999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.656</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.536</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.528</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.447999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.368</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.223999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.176</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$192:$J$204</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1035,11 +1911,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2120456872"/>
-        <c:axId val="2112523736"/>
+        <c:axId val="2113259944"/>
+        <c:axId val="2122293208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2120456872"/>
+        <c:axId val="2113259944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,12 +1925,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112523736"/>
+        <c:crossAx val="2122293208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2112523736"/>
+        <c:axId val="2122293208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1065,7 +1941,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120456872"/>
+        <c:crossAx val="2113259944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1581,6 +2457,806 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Experiment 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$E$84:$E$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.846153846153846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.769230769230769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.615384615384615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.538461538461538</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.461538461538461</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.384615384615384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.307692307692307</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.153846153846153</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0769230769230768</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$84:$J$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Experiment 5</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="660066"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$E$102:$E$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.846153846153846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.769230769230769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.615384615384615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.538461538461538</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.461538461538461</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.384615384615384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.307692307692307</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.153846153846153</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0769230769230768</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$102:$J$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Experiment 6</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$E$120:$E$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.846153846153846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.769230769230769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.615384615384615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.538461538461538</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.461538461538461</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.384615384615384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.307692307692307</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.153846153846153</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0769230769230768</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$120:$J$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Experiment 7</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="19FF37"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$E$138:$E$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.846153846153846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.769230769230769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.615384615384615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.538461538461538</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.461538461538461</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.384615384615384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.307692307692307</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.153846153846153</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0769230769230768</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$138:$J$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>Experiment 8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$E$156:$E$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.846153846153846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.769230769230769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.615384615384615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.538461538461538</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.461538461538461</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.384615384615384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.307692307692307</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.153846153846153</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0769230769230768</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$156:$J$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Experiment 9</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="07F3FF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$E$174:$E$186</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.846153846153846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.769230769230769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.615384615384615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.538461538461538</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.461538461538461</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.384615384615384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.307692307692307</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.153846153846153</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0769230769230768</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$174:$J$186</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:v>Experiment 10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$E$192:$E$204</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.923076923076923</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.846153846153846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.769230769230769</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.692307692307692</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.615384615384615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.538461538461538</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.461538461538461</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.384615384615384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.307692307692307</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.153846153846153</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0769230769230768</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$192:$J$204</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1589,11 +3265,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121893480"/>
-        <c:axId val="2121896504"/>
+        <c:axId val="2116996920"/>
+        <c:axId val="-2104292616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121893480"/>
+        <c:axId val="2116996920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1603,12 +3279,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121896504"/>
+        <c:crossAx val="-2104292616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121896504"/>
+        <c:axId val="-2104292616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1619,7 +3295,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121893480"/>
+        <c:crossAx val="2116996920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2137,6 +3813,755 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Experiment 4</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$F$84:$F$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.81683833415007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.16359238009685</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.14350888035579</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.16066899657005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.17706156313099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.16090568241996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.090351524638</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6254229799344</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.45120187320878</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.24772691011598</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.688222572812375</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.529360865287364</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$84:$J$96</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Experiment 5</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$F$102:$F$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.54525101390749</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8342976353684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.01250426255681</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.02270623949204</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.96816464295311</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.91520129666062</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.89727053984821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.62783449232046</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3238863772389</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.13247092038451</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.978028471326194</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.402179190202272</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$102:$J$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>Experiment 6</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$F$120:$F$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.94638418610266</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.17686923176947</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.17783214475777</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.20722797791856</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.13906545348886</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.11093068251817</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.01244701013802</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9505686308341</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.45248371601233</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.970332336977604</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.880936150764266</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.277839573958309</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$120:$J$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>Experiment 7</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$F$138:$F$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.85180937350629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.91945170224096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.90383458163987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.03785136283693</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.93209877974713</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.83419200298423</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.80368345088428</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.46884226759639</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2092438151071</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.05590659672748</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.551927553456607</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0672215447583068</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$138:$J$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>Experiment 8</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$F$156:$F$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.2848178114669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.50115225936896</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.50115225936896</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.66977873256312</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.69301825699938</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.23945014747678</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.21085608681419</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.11972384583369</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.998030374173846</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.935841553032521</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.721928094887362</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.402179190202272</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$156:$J$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Experiment 9</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$F$174:$F$186</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.81936264169987</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.08620509748812</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.12241963206382</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.07741308818691</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.03483911243094</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.98556057561803</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.56030849271941</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.19232672062985</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1793796225486</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.832636191549581</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.674095105831002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.402179190202272</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$174:$J$186</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:v>Experiment 10</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$F$192:$F$204</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.97746835967822</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.26964721529738</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.22354407637494</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.15578194280104</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.11125534064316</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.01081630791004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.99098770519954</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.66144397194777</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.31511428683238</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.877441581152623</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.772383768202382</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.614822757149069</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>MasterExperiment.csv!$J$192:$J$204</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2145,11 +4570,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2119218616"/>
-        <c:axId val="2119221640"/>
+        <c:axId val="2121528184"/>
+        <c:axId val="2119623560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2119218616"/>
+        <c:axId val="2121528184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2159,12 +4584,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119221640"/>
+        <c:crossAx val="2119623560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2119221640"/>
+        <c:axId val="2119623560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2175,7 +4600,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2119218616"/>
+        <c:crossAx val="2121528184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2701,11 +5126,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121976648"/>
-        <c:axId val="2121836712"/>
+        <c:axId val="2116642024"/>
+        <c:axId val="-2104278664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121976648"/>
+        <c:axId val="2116642024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2715,12 +5140,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121836712"/>
+        <c:crossAx val="-2104278664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121836712"/>
+        <c:axId val="-2104278664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2731,7 +5156,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121976648"/>
+        <c:crossAx val="2116642024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2763,10 +5188,10 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2794,9 +5219,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2820,15 +5245,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2852,15 +5277,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3208,8 +5633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J726"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="M186" sqref="M186"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7468,333 +9893,450 @@
       </c>
     </row>
     <row r="173" spans="1:10">
-      <c r="A173" t="s">
+      <c r="A173" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B173" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C173" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D173" t="s">
+      <c r="D173" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F173" t="s">
+      <c r="F173" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G173" t="s">
+      <c r="G173" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H173" t="s">
+      <c r="H173" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I173" s="1" t="s">
+      <c r="I173" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J173" t="s">
+      <c r="J173" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
-      <c r="A174">
-        <v>0</v>
-      </c>
-      <c r="B174" s="2" t="s">
+    <row r="174" spans="1:10" ht="60">
+      <c r="A174" s="5">
+        <v>0</v>
+      </c>
+      <c r="B174" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D174">
+      <c r="C174" s="15">
+        <v>4</v>
+      </c>
+      <c r="D174" s="5">
         <v>0.99199999999999999</v>
       </c>
-      <c r="E174">
+      <c r="E174" s="5">
         <v>0.92307692307692302</v>
       </c>
-      <c r="F174">
+      <c r="F174" s="5">
         <v>1.8193626416998701</v>
       </c>
-      <c r="G174">
+      <c r="G174" s="5">
         <v>2.13393756609491</v>
       </c>
-      <c r="H174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:10">
-      <c r="A175">
+      <c r="H174" s="5">
+        <v>0</v>
+      </c>
+      <c r="I174" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J174" s="5">
         <v>1</v>
       </c>
-      <c r="B175" s="2">
+    </row>
+    <row r="175" spans="1:10" ht="30">
+      <c r="A175" s="5">
+        <v>1</v>
+      </c>
+      <c r="B175" s="6">
         <v>3</v>
       </c>
-      <c r="D175">
+      <c r="C175" s="5">
+        <v>3</v>
+      </c>
+      <c r="D175" s="5">
         <v>0.91200000000000003</v>
       </c>
-      <c r="E175">
+      <c r="E175" s="5">
         <v>0.84615384615384603</v>
       </c>
-      <c r="F175">
+      <c r="F175" s="5">
         <v>2.0862050974881199</v>
       </c>
-      <c r="G175">
+      <c r="G175" s="5">
         <v>2.2577560641285102</v>
       </c>
-      <c r="H175">
-        <v>0</v>
+      <c r="H175" s="5">
+        <v>0</v>
+      </c>
+      <c r="I175" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J175" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="176" spans="1:10">
-      <c r="A176">
+      <c r="A176" s="5">
         <v>2</v>
       </c>
-      <c r="B176" s="2">
+      <c r="B176" s="6">
         <v>11</v>
       </c>
-      <c r="D176">
+      <c r="C176" s="5">
+        <v>3</v>
+      </c>
+      <c r="D176" s="5">
         <v>0.88800000000000001</v>
       </c>
-      <c r="E176">
+      <c r="E176" s="5">
         <v>0.76923076923076905</v>
       </c>
-      <c r="F176">
+      <c r="F176" s="5">
         <v>2.1224196320638198</v>
       </c>
-      <c r="G176">
+      <c r="G176" s="5">
         <v>2.2577560641285102</v>
       </c>
-      <c r="H176">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10">
-      <c r="A177">
+      <c r="H176" s="5">
+        <v>0</v>
+      </c>
+      <c r="I176" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J176" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" ht="45">
+      <c r="A177" s="5">
         <v>3</v>
       </c>
-      <c r="B177" s="2">
+      <c r="B177" s="6">
         <v>10</v>
       </c>
-      <c r="D177">
+      <c r="C177" s="5">
+        <v>3</v>
+      </c>
+      <c r="D177" s="5">
         <v>0.84</v>
       </c>
-      <c r="E177">
+      <c r="E177" s="5">
         <v>0.69230769230769196</v>
       </c>
-      <c r="F177">
+      <c r="F177" s="5">
         <v>2.0774130881869102</v>
       </c>
-      <c r="G177">
+      <c r="G177" s="5">
         <v>2.1619781796795499</v>
       </c>
-      <c r="H177">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10">
-      <c r="A178">
+      <c r="H177" s="5">
+        <v>0</v>
+      </c>
+      <c r="I177" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J177" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" ht="45">
+      <c r="A178" s="5">
         <v>4</v>
       </c>
-      <c r="B178" s="2">
+      <c r="B178" s="6">
         <v>6</v>
       </c>
-      <c r="D178">
+      <c r="C178" s="5">
+        <v>3</v>
+      </c>
+      <c r="D178" s="5">
         <v>0.68799999999999994</v>
       </c>
-      <c r="E178">
+      <c r="E178" s="5">
         <v>0.61538461538461497</v>
       </c>
-      <c r="F178">
+      <c r="F178" s="5">
         <v>2.03483911243094</v>
       </c>
-      <c r="G178">
+      <c r="G178" s="5">
         <v>2.0381596816459502</v>
       </c>
-      <c r="H178">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10">
-      <c r="A179">
+      <c r="H178" s="5">
+        <v>0</v>
+      </c>
+      <c r="I178" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J178" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" ht="45">
+      <c r="A179" s="5">
         <v>5</v>
       </c>
-      <c r="B179" s="2">
+      <c r="B179" s="6">
         <v>7</v>
       </c>
-      <c r="D179">
+      <c r="C179" s="5">
+        <v>3</v>
+      </c>
+      <c r="D179" s="5">
         <v>0.54400000000000004</v>
       </c>
-      <c r="E179">
+      <c r="E179" s="5">
         <v>0.53846153846153799</v>
       </c>
-      <c r="F179">
+      <c r="F179" s="5">
         <v>1.9855605756180299</v>
       </c>
-      <c r="G179">
+      <c r="G179" s="5">
         <v>1.9877733714879799</v>
       </c>
-      <c r="H179">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180" spans="1:10">
-      <c r="A180">
+      <c r="H179" s="5">
+        <v>0</v>
+      </c>
+      <c r="I179" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J179" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" ht="30">
+      <c r="A180" s="5">
         <v>6</v>
       </c>
-      <c r="B180" s="2">
+      <c r="B180" s="6">
         <v>4</v>
       </c>
-      <c r="D180">
+      <c r="C180" s="5">
+        <v>3</v>
+      </c>
+      <c r="D180" s="5">
         <v>0.42399999999999999</v>
       </c>
-      <c r="E180">
+      <c r="E180" s="5">
         <v>0.46153846153846101</v>
       </c>
-      <c r="F180">
+      <c r="F180" s="5">
         <v>1.56030849271941</v>
       </c>
-      <c r="G180">
+      <c r="G180" s="5">
         <v>1.66918033686673</v>
       </c>
-      <c r="H180">
-        <v>0</v>
+      <c r="H180" s="5">
+        <v>0</v>
+      </c>
+      <c r="I180" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J180" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="181" spans="1:10">
-      <c r="A181">
+      <c r="A181" s="5">
         <v>7</v>
       </c>
-      <c r="B181" s="2">
+      <c r="B181" s="6">
         <v>8</v>
       </c>
-      <c r="D181">
+      <c r="C181" s="5">
+        <v>3</v>
+      </c>
+      <c r="D181" s="5">
         <v>0.30399999999999999</v>
       </c>
-      <c r="E181">
+      <c r="E181" s="5">
         <v>0.38461538461538403</v>
       </c>
-      <c r="F181">
+      <c r="F181" s="5">
         <v>1.19232672062985</v>
       </c>
-      <c r="G181">
+      <c r="G181" s="5">
         <v>1.4885252948977401</v>
       </c>
-      <c r="H181">
-        <v>0</v>
+      <c r="H181" s="5">
+        <v>0</v>
+      </c>
+      <c r="I181" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J181" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="182" spans="1:10">
-      <c r="A182">
+      <c r="A182" s="5">
         <v>8</v>
       </c>
-      <c r="B182" s="2">
+      <c r="B182" s="6">
         <v>12</v>
       </c>
-      <c r="D182">
+      <c r="C182" s="5">
+        <v>3</v>
+      </c>
+      <c r="D182" s="5">
         <v>0.29599999999999999</v>
       </c>
-      <c r="E182">
+      <c r="E182" s="5">
         <v>0.30769230769230699</v>
       </c>
-      <c r="F182">
+      <c r="F182" s="5">
         <v>1.1793796225486</v>
       </c>
-      <c r="G182">
+      <c r="G182" s="5">
         <v>1.3520301017579499</v>
       </c>
-      <c r="H182">
-        <v>0</v>
+      <c r="H182" s="5">
+        <v>0</v>
+      </c>
+      <c r="I182" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J182" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:10">
-      <c r="A183">
+      <c r="A183" s="5">
         <v>9</v>
       </c>
-      <c r="B183" s="2">
+      <c r="B183" s="6">
         <v>5</v>
       </c>
-      <c r="D183">
+      <c r="C183" s="5">
+        <v>3</v>
+      </c>
+      <c r="D183" s="5">
         <v>0.152</v>
       </c>
-      <c r="E183">
+      <c r="E183" s="5">
         <v>0.23076923076923</v>
       </c>
-      <c r="F183">
+      <c r="F183" s="5">
         <v>0.83263619154958102</v>
       </c>
-      <c r="G183">
+      <c r="G183" s="5">
         <v>1.14511041438158</v>
       </c>
-      <c r="H183">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184" spans="1:10">
-      <c r="A184">
+      <c r="H183" s="5">
+        <v>0</v>
+      </c>
+      <c r="I183" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J183" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" ht="30">
+      <c r="A184" s="5">
         <v>10</v>
       </c>
-      <c r="B184" s="2">
+      <c r="B184" s="6">
         <v>1</v>
       </c>
-      <c r="D184">
+      <c r="C184" s="5">
+        <v>1</v>
+      </c>
+      <c r="D184" s="5">
         <v>0.128</v>
       </c>
-      <c r="E184">
+      <c r="E184" s="5">
         <v>0.15384615384615299</v>
       </c>
-      <c r="F184">
+      <c r="F184" s="5">
         <v>0.67409510583100196</v>
       </c>
-      <c r="G184">
+      <c r="G184" s="5">
         <v>0.77322834852491695</v>
       </c>
-      <c r="H184">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:10">
-      <c r="A185">
+      <c r="H184" s="5">
+        <v>0</v>
+      </c>
+      <c r="I184" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J184" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" ht="30">
+      <c r="A185" s="5">
         <v>11</v>
       </c>
-      <c r="B185" s="2">
+      <c r="B185" s="6">
         <v>2</v>
       </c>
-      <c r="D185">
+      <c r="C185" s="5">
+        <v>1</v>
+      </c>
+      <c r="D185" s="5">
         <v>7.9999999999999905E-2</v>
       </c>
-      <c r="E185">
+      <c r="E185" s="5">
         <v>7.6923076923076802E-2</v>
       </c>
-      <c r="F185">
+      <c r="F185" s="5">
         <v>0.402179190202272</v>
       </c>
-      <c r="G185">
+      <c r="G185" s="5">
         <v>0.391243563629255</v>
       </c>
-      <c r="H185">
+      <c r="H185" s="5">
+        <v>0</v>
+      </c>
+      <c r="I185" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J185" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:10">
-      <c r="A186">
+      <c r="A186" s="5">
         <v>12</v>
       </c>
-      <c r="B186" s="2">
+      <c r="B186" s="6">
         <v>9</v>
       </c>
-      <c r="D186">
-        <v>0</v>
-      </c>
-      <c r="E186">
-        <v>0</v>
-      </c>
-      <c r="F186">
-        <v>0</v>
-      </c>
-      <c r="G186">
-        <v>0</v>
-      </c>
-      <c r="H186">
+      <c r="C186" s="5">
+        <v>1</v>
+      </c>
+      <c r="D186" s="5">
+        <v>0</v>
+      </c>
+      <c r="E186" s="5">
+        <v>0</v>
+      </c>
+      <c r="F186" s="5">
+        <v>0</v>
+      </c>
+      <c r="G186" s="5">
+        <v>0</v>
+      </c>
+      <c r="H186" s="5">
+        <v>0</v>
+      </c>
+      <c r="I186" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J186" s="5">
         <v>0</v>
       </c>
     </row>
@@ -7815,337 +10357,454 @@
       </c>
     </row>
     <row r="191" spans="1:10">
-      <c r="A191" t="s">
+      <c r="A191" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B191" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E191" t="s">
+      <c r="E191" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F191" t="s">
+      <c r="F191" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G191" t="s">
+      <c r="G191" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H191" t="s">
+      <c r="H191" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I191" s="1" t="s">
+      <c r="I191" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J191" t="s">
+      <c r="J191" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
-      <c r="A192">
-        <v>0</v>
-      </c>
-      <c r="B192" s="2" t="s">
+    <row r="192" spans="1:10" ht="30">
+      <c r="A192" s="5">
+        <v>0</v>
+      </c>
+      <c r="B192" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D192">
+      <c r="C192" s="5">
+        <v>3</v>
+      </c>
+      <c r="D192" s="5">
         <v>0.99199999999999999</v>
       </c>
-      <c r="E192">
+      <c r="E192" s="5">
         <v>0.92307692307692302</v>
       </c>
-      <c r="F192">
+      <c r="F192" s="5">
         <v>1.9774683596782201</v>
       </c>
-      <c r="G192">
+      <c r="G192" s="5">
         <v>2.2373974097831</v>
       </c>
-      <c r="H192">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8">
-      <c r="A193">
+      <c r="H192" s="5">
+        <v>0</v>
+      </c>
+      <c r="I192" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J192" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10">
+      <c r="A193" s="5">
         <v>1</v>
       </c>
-      <c r="B193" s="2">
+      <c r="B193" s="6">
         <v>7</v>
       </c>
-      <c r="D193">
+      <c r="C193" s="5">
+        <v>3</v>
+      </c>
+      <c r="D193" s="5">
         <v>0.84799999999999998</v>
       </c>
-      <c r="E193">
+      <c r="E193" s="5">
         <v>0.84615384615384603</v>
       </c>
-      <c r="F193">
+      <c r="F193" s="5">
         <v>2.2696472152973799</v>
       </c>
-      <c r="G193">
+      <c r="G193" s="5">
         <v>2.2954656791802899</v>
       </c>
-      <c r="H193">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8">
-      <c r="A194">
+      <c r="H193" s="5">
+        <v>0</v>
+      </c>
+      <c r="I193" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J193" s="5">
         <v>2</v>
       </c>
-      <c r="B194" s="2">
+    </row>
+    <row r="194" spans="1:10" ht="30">
+      <c r="A194" s="5">
+        <v>2</v>
+      </c>
+      <c r="B194" s="6">
         <v>4</v>
       </c>
-      <c r="D194">
+      <c r="C194" s="5">
+        <v>1</v>
+      </c>
+      <c r="D194" s="5">
         <v>0.72799999999999998</v>
       </c>
-      <c r="E194">
+      <c r="E194" s="5">
         <v>0.76923076923076905</v>
       </c>
-      <c r="F194">
+      <c r="F194" s="5">
         <v>2.2235440763749401</v>
       </c>
-      <c r="G194">
+      <c r="G194" s="5">
         <v>2.2954656791802899</v>
       </c>
-      <c r="H194">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8">
-      <c r="A195">
+      <c r="H194" s="5">
+        <v>0</v>
+      </c>
+      <c r="I194" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J194" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" ht="30">
+      <c r="A195" s="5">
         <v>3</v>
       </c>
-      <c r="B195" s="2">
+      <c r="B195" s="6">
         <v>2</v>
       </c>
-      <c r="D195">
+      <c r="C195" s="5">
+        <v>2</v>
+      </c>
+      <c r="D195" s="5">
         <v>0.67999999999999905</v>
       </c>
-      <c r="E195">
+      <c r="E195" s="5">
         <v>0.69230769230769196</v>
       </c>
-      <c r="F195">
+      <c r="F195" s="5">
         <v>2.1557819428010401</v>
       </c>
-      <c r="G195">
+      <c r="G195" s="5">
         <v>2.2577560641285102</v>
       </c>
-      <c r="H195">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8">
-      <c r="A196">
+      <c r="H195" s="5">
+        <v>0</v>
+      </c>
+      <c r="I195" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="J195" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" ht="30">
+      <c r="A196" s="5">
         <v>4</v>
       </c>
-      <c r="B196" s="2">
+      <c r="B196" s="6">
         <v>1</v>
       </c>
-      <c r="D196">
+      <c r="C196" s="5">
+        <v>1</v>
+      </c>
+      <c r="D196" s="5">
         <v>0.65600000000000003</v>
       </c>
-      <c r="E196">
+      <c r="E196" s="5">
         <v>0.61538461538461497</v>
       </c>
-      <c r="F196">
+      <c r="F196" s="5">
         <v>2.1112553406431598</v>
       </c>
-      <c r="G196">
+      <c r="G196" s="5">
         <v>2.13393756609491</v>
       </c>
-      <c r="H196">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8">
-      <c r="A197">
+      <c r="H196" s="5">
+        <v>0</v>
+      </c>
+      <c r="I196" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J196" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10">
+      <c r="A197" s="5">
         <v>5</v>
       </c>
-      <c r="B197" s="2">
+      <c r="B197" s="6">
         <v>8</v>
       </c>
-      <c r="D197">
+      <c r="C197" s="5">
+        <v>1</v>
+      </c>
+      <c r="D197" s="5">
         <v>0.53600000000000003</v>
       </c>
-      <c r="E197">
+      <c r="E197" s="5">
         <v>0.53846153846153799</v>
       </c>
-      <c r="F197">
+      <c r="F197" s="5">
         <v>2.0108163079100398</v>
       </c>
-      <c r="G197">
+      <c r="G197" s="5">
         <v>2.0458416408851701</v>
       </c>
-      <c r="H197">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8">
-      <c r="A198">
+      <c r="H197" s="5">
+        <v>0</v>
+      </c>
+      <c r="I197" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J197" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10">
+      <c r="A198" s="5">
         <v>6</v>
       </c>
-      <c r="B198" s="2">
+      <c r="B198" s="6">
         <v>12</v>
       </c>
-      <c r="D198">
+      <c r="C198" s="5">
+        <v>1</v>
+      </c>
+      <c r="D198" s="5">
         <v>0.52800000000000002</v>
       </c>
-      <c r="E198">
+      <c r="E198" s="5">
         <v>0.46153846153846101</v>
       </c>
-      <c r="F198">
+      <c r="F198" s="5">
         <v>1.9909877051995399</v>
       </c>
-      <c r="G198">
+      <c r="G198" s="5">
         <v>1.88109476011007</v>
       </c>
-      <c r="H198">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8">
-      <c r="A199">
+      <c r="H198" s="5">
+        <v>0</v>
+      </c>
+      <c r="I198" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J198" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10">
+      <c r="A199" s="5">
         <v>7</v>
       </c>
-      <c r="B199" s="2">
+      <c r="B199" s="6">
         <v>9</v>
       </c>
-      <c r="D199">
+      <c r="C199" s="5">
+        <v>1</v>
+      </c>
+      <c r="D199" s="5">
         <v>0.44799999999999901</v>
       </c>
-      <c r="E199">
+      <c r="E199" s="5">
         <v>0.38461538461538403</v>
       </c>
-      <c r="F199">
+      <c r="F199" s="5">
         <v>1.66144397194777</v>
       </c>
-      <c r="G199">
+      <c r="G199" s="5">
         <v>1.54659356429493</v>
       </c>
-      <c r="H199">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8">
-      <c r="A200">
+      <c r="H199" s="5">
+        <v>0</v>
+      </c>
+      <c r="I199" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J199" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" ht="45">
+      <c r="A200" s="5">
         <v>8</v>
       </c>
-      <c r="B200" s="2">
+      <c r="B200" s="6">
         <v>3</v>
       </c>
-      <c r="D200">
+      <c r="C200" s="5">
+        <v>1</v>
+      </c>
+      <c r="D200" s="5">
         <v>0.36799999999999999</v>
       </c>
-      <c r="E200">
+      <c r="E200" s="5">
         <v>0.30769230769230699</v>
       </c>
-      <c r="F200">
+      <c r="F200" s="5">
         <v>1.31511428683238</v>
       </c>
-      <c r="G200">
+      <c r="G200" s="5">
         <v>1.1981839479117899</v>
       </c>
-      <c r="H200">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8">
-      <c r="A201">
+      <c r="H200" s="5">
+        <v>0</v>
+      </c>
+      <c r="I200" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="J200" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10">
+      <c r="A201" s="5">
         <v>9</v>
       </c>
-      <c r="B201" s="2">
+      <c r="B201" s="6">
         <v>5</v>
       </c>
-      <c r="D201">
+      <c r="C201" s="5">
+        <v>1</v>
+      </c>
+      <c r="D201" s="5">
         <v>0.22399999999999901</v>
       </c>
-      <c r="E201">
+      <c r="E201" s="5">
         <v>0.23076923076923</v>
       </c>
-      <c r="F201">
+      <c r="F201" s="5">
         <v>0.87744158115262305</v>
       </c>
-      <c r="G201">
+      <c r="G201" s="5">
         <v>0.99126426053542804</v>
       </c>
-      <c r="H201">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8">
-      <c r="A202">
+      <c r="H201" s="5">
+        <v>0</v>
+      </c>
+      <c r="I201" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J201" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10">
+      <c r="A202" s="5">
         <v>10</v>
       </c>
-      <c r="B202" s="2">
+      <c r="B202" s="6">
         <v>10</v>
       </c>
-      <c r="D202">
+      <c r="C202" s="5">
+        <v>1</v>
+      </c>
+      <c r="D202" s="5">
         <v>0.17599999999999999</v>
       </c>
-      <c r="E202">
+      <c r="E202" s="5">
         <v>0.15384615384615299</v>
       </c>
-      <c r="F202">
+      <c r="F202" s="5">
         <v>0.77238376820238197</v>
       </c>
-      <c r="G202">
+      <c r="G202" s="5">
         <v>0.77322834852491695</v>
       </c>
-      <c r="H202">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8">
-      <c r="A203">
+      <c r="H202" s="5">
+        <v>0</v>
+      </c>
+      <c r="I202" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J202" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10">
+      <c r="A203" s="5">
         <v>11</v>
       </c>
-      <c r="B203" s="2">
+      <c r="B203" s="6">
         <v>11</v>
       </c>
-      <c r="D203">
+      <c r="C203" s="5">
+        <v>1</v>
+      </c>
+      <c r="D203" s="5">
         <v>0.152</v>
       </c>
-      <c r="E203">
+      <c r="E203" s="5">
         <v>7.6923076923076802E-2</v>
       </c>
-      <c r="F203">
+      <c r="F203" s="5">
         <v>0.61482275714906898</v>
       </c>
-      <c r="G203">
+      <c r="G203" s="5">
         <v>0.391243563629255</v>
       </c>
-      <c r="H203">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8">
-      <c r="A204">
+      <c r="H203" s="5">
+        <v>0</v>
+      </c>
+      <c r="I203" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J203" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" ht="30">
+      <c r="A204" s="5">
         <v>12</v>
       </c>
-      <c r="B204" s="2">
+      <c r="B204" s="6">
         <v>6</v>
       </c>
-      <c r="D204">
-        <v>0</v>
-      </c>
-      <c r="E204">
-        <v>0</v>
-      </c>
-      <c r="F204">
-        <v>0</v>
-      </c>
-      <c r="G204">
-        <v>0</v>
-      </c>
-      <c r="H204">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8">
+      <c r="C204" s="5">
+        <v>1</v>
+      </c>
+      <c r="D204" s="5">
+        <v>0</v>
+      </c>
+      <c r="E204" s="5">
+        <v>0</v>
+      </c>
+      <c r="F204" s="5">
+        <v>0</v>
+      </c>
+      <c r="G204" s="5">
+        <v>0</v>
+      </c>
+      <c r="H204" s="5">
+        <v>0</v>
+      </c>
+      <c r="I204" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J204" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10">
       <c r="A207" s="9" t="s">
         <v>7</v>
       </c>
@@ -8153,7 +10812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:10">
       <c r="A208" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
added class 4 table
</commit_message>
<xml_diff>
--- a/project1/MasterExperiment.xlsx
+++ b/project1/MasterExperiment.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33620" yWindow="0" windowWidth="33580" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="-33620" yWindow="0" windowWidth="33580" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MasterExperiment.csv" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Class 4 table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="203">
   <si>
     <t>Your</t>
   </si>
@@ -397,9 +397,6 @@
     <t>This one is very beutifull complex structure that combines patterns from classes 1,2 and 3.</t>
   </si>
   <si>
-    <t>This one is interesting. It lookes like chaotic structure of different triangle shaped patterns. But there is another pattern on a top of it that goes from the top to the bottom, that has another color and it changes shapes as well. So this is in between classes 3 and 4 but closer to 4.</t>
-  </si>
-  <si>
     <t>This one is very similar but there is nothing complex, only chaotic triangle structures</t>
   </si>
   <si>
@@ -467,9 +464,6 @@
   </si>
   <si>
     <t>There chaotic triangle structures with some another complex structure going through it</t>
-  </si>
-  <si>
-    <t>This one has less chaos and actually got some perodicity. But it's really hard to say, it is very complex</t>
   </si>
   <si>
     <t>Chaotic pattern consisting of larger triangle structures, there are some line-liketiny structs, but I would still give it class 3</t>
@@ -609,6 +603,33 @@
   <si>
     <t>Number of experiments</t>
   </si>
+  <si>
+    <t>This structure is very chaotic. And even though there are some kind of periodic line in there, they are very small, and also tend to be in random order. It is very complex, really hard to tell. It's is in between class 3 and 4 , but closer to 4</t>
+  </si>
+  <si>
+    <t>This one has less chaos and actually got some perodicity. But it's really hard to say. It's kind of moving towards class 4 but not there yet</t>
+  </si>
+  <si>
+    <t>This one is interesting. It lookes like chaotic structure of different triangle shaped patterns. But there is another pattern on a top of it that goes from the top to the bottom, that has another color and it changes shapes as well. So this is in between classes 3 and 4 but closer to 3 any way.</t>
+  </si>
+  <si>
+    <t>same but closer to class 3</t>
+  </si>
+  <si>
+    <t>same but closer to 4 again</t>
+  </si>
+  <si>
+    <t>Experiment #</t>
+  </si>
+  <si>
+    <t>Step #</t>
+  </si>
+  <si>
+    <t>Possition zeroed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Class #</t>
+  </si>
 </sst>
 </file>
 
@@ -654,7 +675,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -691,8 +712,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4D79B"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -737,8 +764,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="297">
+  <cellStyleXfs count="339">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1036,8 +1100,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1081,8 +1187,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="297">
+  <cellStyles count="339">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1231,6 +1354,27 @@
     <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1379,6 +1523,27 @@
     <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2556,10 +2721,10 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.0</c:v>
@@ -3685,7 +3850,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0</c:v>
@@ -4384,7 +4549,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.0</c:v>
@@ -7248,10 +7413,10 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.0</c:v>
@@ -8377,7 +8542,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0</c:v>
@@ -9076,7 +9241,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.0</c:v>
@@ -11812,10 +11977,10 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.0</c:v>
@@ -12941,7 +13106,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0</c:v>
@@ -13640,7 +13805,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.0</c:v>
@@ -16504,10 +16669,10 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.0</c:v>
@@ -17633,7 +17798,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0</c:v>
@@ -18332,7 +18497,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.0</c:v>
@@ -21196,10 +21361,10 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.0</c:v>
@@ -22325,7 +22490,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2.0</c:v>
@@ -23024,7 +23189,7 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.0</c:v>
@@ -25187,8 +25352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J726"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="R130" sqref="R130"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="L701" sqref="L701"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25253,7 +25418,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B7" s="26">
         <v>40</v>
@@ -29621,8 +29786,8 @@
       <c r="B178" s="6">
         <v>6</v>
       </c>
-      <c r="C178" s="5">
-        <v>3</v>
+      <c r="C178" s="10">
+        <v>4</v>
       </c>
       <c r="D178" s="5">
         <v>0.68799999999999994</v>
@@ -29643,18 +29808,18 @@
         <v>75</v>
       </c>
       <c r="J178" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10" ht="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" ht="60">
       <c r="A179" s="5">
         <v>5</v>
       </c>
       <c r="B179" s="6">
         <v>7</v>
       </c>
-      <c r="C179" s="5">
-        <v>3</v>
+      <c r="C179" s="10">
+        <v>4</v>
       </c>
       <c r="D179" s="5">
         <v>0.54400000000000004</v>
@@ -29672,10 +29837,10 @@
         <v>0</v>
       </c>
       <c r="I179" s="7" t="s">
-        <v>76</v>
+        <v>194</v>
       </c>
       <c r="J179" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:10" ht="30">
@@ -33320,7 +33485,7 @@
         <v>0</v>
       </c>
       <c r="I321" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J321" s="5">
         <v>2</v>
@@ -34165,8 +34330,8 @@
       <c r="B355" s="6">
         <v>10</v>
       </c>
-      <c r="C355" s="10">
-        <v>4</v>
+      <c r="C355" s="24">
+        <v>3</v>
       </c>
       <c r="D355" s="5">
         <v>0.94399999999999995</v>
@@ -34184,10 +34349,10 @@
         <v>0</v>
       </c>
       <c r="I355" s="7" t="s">
-        <v>125</v>
+        <v>196</v>
       </c>
       <c r="J355" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="356" spans="1:10" ht="30">
@@ -34216,7 +34381,7 @@
         <v>0</v>
       </c>
       <c r="I356" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J356" s="5">
         <v>2</v>
@@ -34248,7 +34413,7 @@
         <v>0</v>
       </c>
       <c r="I357" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J357" s="5">
         <v>0</v>
@@ -34280,7 +34445,7 @@
         <v>0</v>
       </c>
       <c r="I358" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J358" s="5">
         <v>2</v>
@@ -34376,7 +34541,7 @@
         <v>0</v>
       </c>
       <c r="I361" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J361" s="5">
         <v>2</v>
@@ -34616,7 +34781,7 @@
         <v>0</v>
       </c>
       <c r="I372" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J372" s="5">
         <v>2</v>
@@ -34648,7 +34813,7 @@
         <v>0</v>
       </c>
       <c r="I373" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J373" s="5">
         <v>1</v>
@@ -35080,7 +35245,7 @@
         <v>0</v>
       </c>
       <c r="I390" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J390" s="5">
         <v>2</v>
@@ -35112,7 +35277,7 @@
         <v>0</v>
       </c>
       <c r="I391" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J391" s="5">
         <v>2</v>
@@ -35144,7 +35309,7 @@
         <v>0</v>
       </c>
       <c r="I392" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J392" s="5">
         <v>2</v>
@@ -35240,7 +35405,7 @@
         <v>0</v>
       </c>
       <c r="I395" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J395" s="5">
         <v>0</v>
@@ -35272,7 +35437,7 @@
         <v>0</v>
       </c>
       <c r="I396" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J396" s="5">
         <v>0</v>
@@ -35304,7 +35469,7 @@
         <v>0</v>
       </c>
       <c r="I397" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J397" s="5">
         <v>0</v>
@@ -35544,7 +35709,7 @@
         <v>0</v>
       </c>
       <c r="I408" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J408" s="5">
         <v>1</v>
@@ -35608,7 +35773,7 @@
         <v>0</v>
       </c>
       <c r="I410" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J410" s="5">
         <v>2</v>
@@ -35736,7 +35901,7 @@
         <v>0</v>
       </c>
       <c r="I414" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J414" s="5">
         <v>2</v>
@@ -35768,7 +35933,7 @@
         <v>0</v>
       </c>
       <c r="I415" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J415" s="5">
         <v>0</v>
@@ -35800,7 +35965,7 @@
         <v>0</v>
       </c>
       <c r="I416" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J416" s="5">
         <v>0</v>
@@ -36116,7 +36281,7 @@
         <v>0</v>
       </c>
       <c r="I429" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J429" s="5">
         <v>2</v>
@@ -36180,7 +36345,7 @@
         <v>0</v>
       </c>
       <c r="I431" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J431" s="5">
         <v>2</v>
@@ -36212,7 +36377,7 @@
         <v>0</v>
       </c>
       <c r="I432" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J432" s="5">
         <v>0</v>
@@ -36484,7 +36649,7 @@
         <v>0</v>
       </c>
       <c r="I444" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J444" s="5">
         <v>2</v>
@@ -36580,7 +36745,7 @@
         <v>0</v>
       </c>
       <c r="I447" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J447" s="5">
         <v>2</v>
@@ -36612,7 +36777,7 @@
         <v>0</v>
       </c>
       <c r="I448" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J448" s="5">
         <v>1</v>
@@ -37114,15 +37279,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="468" spans="1:10" ht="30">
+    <row r="468" spans="1:10" ht="45">
       <c r="A468" s="5">
         <v>6</v>
       </c>
       <c r="B468" s="6">
         <v>7</v>
       </c>
-      <c r="C468" s="10">
-        <v>4</v>
+      <c r="C468" s="24">
+        <v>3</v>
       </c>
       <c r="D468" s="5">
         <v>0.55200000000000005</v>
@@ -37140,10 +37305,10 @@
         <v>0</v>
       </c>
       <c r="I468" s="7" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="J468" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="469" spans="1:10">
@@ -37172,7 +37337,7 @@
         <v>0</v>
       </c>
       <c r="I469" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J469" s="5">
         <v>2</v>
@@ -37204,7 +37369,7 @@
         <v>0</v>
       </c>
       <c r="I470" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J470" s="5">
         <v>1</v>
@@ -37268,7 +37433,7 @@
         <v>0</v>
       </c>
       <c r="I472" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J472" s="5">
         <v>0</v>
@@ -37300,7 +37465,7 @@
         <v>0</v>
       </c>
       <c r="I473" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J473" s="5">
         <v>0</v>
@@ -37412,7 +37577,7 @@
         <v>0</v>
       </c>
       <c r="I480" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J480" s="5">
         <v>2</v>
@@ -37476,7 +37641,7 @@
         <v>0</v>
       </c>
       <c r="I482" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J482" s="5">
         <v>0</v>
@@ -37636,7 +37801,7 @@
         <v>0</v>
       </c>
       <c r="I487" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J487" s="5">
         <v>0</v>
@@ -37970,7 +38135,7 @@
         <v>0</v>
       </c>
       <c r="I501" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J501" s="5">
         <v>2</v>
@@ -38002,7 +38167,7 @@
         <v>0</v>
       </c>
       <c r="I502" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J502" s="5">
         <v>2</v>
@@ -38402,7 +38567,7 @@
         <v>0</v>
       </c>
       <c r="I518" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J518" s="5">
         <v>2</v>
@@ -38434,7 +38599,7 @@
         <v>0</v>
       </c>
       <c r="I519" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J519" s="5">
         <v>2</v>
@@ -38562,7 +38727,7 @@
         <v>0</v>
       </c>
       <c r="I523" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J523" s="5">
         <v>0</v>
@@ -38594,7 +38759,7 @@
         <v>0</v>
       </c>
       <c r="I524" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J524" s="5">
         <v>0</v>
@@ -38802,7 +38967,7 @@
         <v>0</v>
       </c>
       <c r="I534" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J534" s="5">
         <v>2</v>
@@ -38834,7 +38999,7 @@
         <v>0</v>
       </c>
       <c r="I535" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J535" s="5">
         <v>2</v>
@@ -39426,7 +39591,7 @@
         <v>0</v>
       </c>
       <c r="I557" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J557" s="5">
         <v>2</v>
@@ -39458,7 +39623,7 @@
         <v>0</v>
       </c>
       <c r="I558" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J558" s="5">
         <v>2</v>
@@ -39490,7 +39655,7 @@
         <v>0</v>
       </c>
       <c r="I559" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J559" s="5">
         <v>2</v>
@@ -39554,7 +39719,7 @@
         <v>0</v>
       </c>
       <c r="I561" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J561" s="5">
         <v>2</v>
@@ -39586,7 +39751,7 @@
         <v>0</v>
       </c>
       <c r="I562" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J562" s="5">
         <v>0</v>
@@ -39826,7 +39991,7 @@
         <v>0</v>
       </c>
       <c r="I573" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J573" s="5">
         <v>0</v>
@@ -40258,7 +40423,7 @@
         <v>0</v>
       </c>
       <c r="I590" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J590" s="5">
         <v>2</v>
@@ -40658,7 +40823,7 @@
         <v>0</v>
       </c>
       <c r="I606" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J606" s="5">
         <v>0</v>
@@ -40754,7 +40919,7 @@
         <v>0</v>
       </c>
       <c r="I609" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J609" s="5">
         <v>2</v>
@@ -40946,7 +41111,7 @@
         <v>0</v>
       </c>
       <c r="I615" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J615" s="5">
         <v>2</v>
@@ -41122,7 +41287,7 @@
         <v>0</v>
       </c>
       <c r="I624" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J624" s="5">
         <v>2</v>
@@ -41346,7 +41511,7 @@
         <v>0</v>
       </c>
       <c r="I631" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J631" s="5">
         <v>2</v>
@@ -41378,7 +41543,7 @@
         <v>0</v>
       </c>
       <c r="I632" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J632" s="5">
         <v>2</v>
@@ -41442,7 +41607,7 @@
         <v>0</v>
       </c>
       <c r="I634" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J634" s="5">
         <v>2</v>
@@ -41650,7 +41815,7 @@
         <v>0</v>
       </c>
       <c r="I644" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J644" s="5">
         <v>0</v>
@@ -41682,7 +41847,7 @@
         <v>0</v>
       </c>
       <c r="I645" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J645" s="5">
         <v>0</v>
@@ -42050,7 +42215,7 @@
         <v>0</v>
       </c>
       <c r="I660" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J660" s="5">
         <v>2</v>
@@ -42082,7 +42247,7 @@
         <v>0</v>
       </c>
       <c r="I661" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J661" s="5">
         <v>2</v>
@@ -42128,7 +42293,7 @@
         <v>3</v>
       </c>
       <c r="C663" s="15" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D663" s="5">
         <v>0.74399999999999999</v>
@@ -42146,7 +42311,7 @@
         <v>0</v>
       </c>
       <c r="I663" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J663" s="5">
         <v>1</v>
@@ -42178,7 +42343,7 @@
         <v>0</v>
       </c>
       <c r="I664" s="7" t="s">
-        <v>29</v>
+        <v>197</v>
       </c>
       <c r="J664" s="5">
         <v>2</v>
@@ -42192,7 +42357,7 @@
         <v>12</v>
       </c>
       <c r="C665" s="15" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D665" s="5">
         <v>0.59199999999999997</v>
@@ -42210,7 +42375,7 @@
         <v>0</v>
       </c>
       <c r="I665" s="7" t="s">
-        <v>29</v>
+        <v>198</v>
       </c>
       <c r="J665" s="5">
         <v>1</v>
@@ -42242,7 +42407,7 @@
         <v>0</v>
       </c>
       <c r="I666" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J666" s="5">
         <v>2</v>
@@ -42370,7 +42535,7 @@
         <v>0</v>
       </c>
       <c r="I670" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J670" s="5">
         <v>2</v>
@@ -42514,7 +42679,7 @@
         <v>0</v>
       </c>
       <c r="I678" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J678" s="5">
         <v>2</v>
@@ -42546,7 +42711,7 @@
         <v>0</v>
       </c>
       <c r="I679" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J679" s="5">
         <v>0</v>
@@ -42578,7 +42743,7 @@
         <v>0</v>
       </c>
       <c r="I680" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J680" s="5">
         <v>0</v>
@@ -42610,7 +42775,7 @@
         <v>0</v>
       </c>
       <c r="I681" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J681" s="5">
         <v>2</v>
@@ -42642,7 +42807,7 @@
         <v>0</v>
       </c>
       <c r="I682" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J682" s="5">
         <v>2</v>
@@ -42674,7 +42839,7 @@
         <v>0</v>
       </c>
       <c r="I683" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J683" s="5">
         <v>2</v>
@@ -42802,7 +42967,7 @@
         <v>0</v>
       </c>
       <c r="I687" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J687" s="5">
         <v>2</v>
@@ -42978,7 +43143,7 @@
         <v>0</v>
       </c>
       <c r="I696" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J696" s="5">
         <v>2</v>
@@ -43042,7 +43207,7 @@
         <v>0</v>
       </c>
       <c r="I698" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J698" s="5">
         <v>1</v>
@@ -43106,7 +43271,7 @@
         <v>0</v>
       </c>
       <c r="I700" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J700" s="5">
         <v>0</v>
@@ -43442,7 +43607,7 @@
         <v>0</v>
       </c>
       <c r="I714" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J714" s="5">
         <v>0</v>
@@ -43506,7 +43671,7 @@
         <v>0</v>
       </c>
       <c r="I716" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J716" s="5">
         <v>0</v>
@@ -43538,7 +43703,7 @@
         <v>0</v>
       </c>
       <c r="I717" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J717" s="5">
         <v>2</v>
@@ -43698,7 +43863,7 @@
         <v>0</v>
       </c>
       <c r="I722" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J722" s="5">
         <v>0</v>
@@ -43846,12 +44011,819 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="53.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="A2" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" ht="70" customHeight="1">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.84615384615384603</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1.8420328973484701</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2.1619781796795499</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="10">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1.9424206646906801</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2.1996877947313198</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="10">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.69230769230769196</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2.1606689965700498</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2.1996877947313198</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="75">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.76923076923076905</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2.0125042625568099</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2.1996877947313198</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="10">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1.9463841861026601</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2.1996877947313198</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45">
+      <c r="A8" s="24">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6">
+        <v>5</v>
+      </c>
+      <c r="D8" s="10">
+        <v>4</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.76</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.69230769230769196</v>
+      </c>
+      <c r="G8" s="5">
+        <v>2.20722797791856</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2.1996877947313198</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45">
+      <c r="A9" s="24">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6">
+        <v>10</v>
+      </c>
+      <c r="D9" s="10">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.504</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1.8036834508842801</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1.8230264907128799</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="60">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.92307692307692302</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1.8193626416998701</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2.13393756609491</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45">
+      <c r="A11" s="24">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6">
+        <v>6</v>
+      </c>
+      <c r="D11" s="10">
+        <v>4</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2.03483911243094</v>
+      </c>
+      <c r="H11" s="5">
+        <v>2.0381596816459502</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="60">
+      <c r="A12" s="24">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6">
+        <v>7</v>
+      </c>
+      <c r="D12" s="10">
+        <v>4</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1.9855605756180299</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1.9877733714879799</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="60">
+      <c r="A13" s="24">
+        <v>11</v>
+      </c>
+      <c r="B13" s="27">
+        <v>2</v>
+      </c>
+      <c r="C13" s="28">
+        <v>10</v>
+      </c>
+      <c r="D13" s="29">
+        <v>4</v>
+      </c>
+      <c r="E13" s="30">
+        <v>0.92</v>
+      </c>
+      <c r="F13" s="30">
+        <v>0.76923076899999998</v>
+      </c>
+      <c r="G13" s="30">
+        <v>1.6348058110000001</v>
+      </c>
+      <c r="H13" s="30">
+        <v>1.8339272179999999</v>
+      </c>
+      <c r="I13" s="30">
+        <v>0</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="60">
+      <c r="A14" s="24">
+        <v>14</v>
+      </c>
+      <c r="B14" s="27">
+        <v>6</v>
+      </c>
+      <c r="C14" s="28">
+        <v>8</v>
+      </c>
+      <c r="D14" s="29">
+        <v>4</v>
+      </c>
+      <c r="E14" s="30">
+        <v>0.48</v>
+      </c>
+      <c r="F14" s="30">
+        <v>0.46153846199999998</v>
+      </c>
+      <c r="G14" s="30">
+        <v>1.8028388829999999</v>
+      </c>
+      <c r="H14" s="30">
+        <v>1.8810947600000001</v>
+      </c>
+      <c r="I14" s="30">
+        <v>0</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="24">
+        <v>14</v>
+      </c>
+      <c r="B15" s="32">
+        <v>7</v>
+      </c>
+      <c r="C15" s="33">
+        <v>4</v>
+      </c>
+      <c r="D15" s="34">
+        <v>4</v>
+      </c>
+      <c r="E15" s="35">
+        <v>0.36</v>
+      </c>
+      <c r="F15" s="35">
+        <v>0.38461538499999998</v>
+      </c>
+      <c r="G15" s="35">
+        <v>1.4508662649999999</v>
+      </c>
+      <c r="H15" s="35">
+        <v>1.7004397179999999</v>
+      </c>
+      <c r="I15" s="35">
+        <v>0</v>
+      </c>
+      <c r="J15" s="36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="45">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16" s="27">
+        <v>0</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="29">
+        <v>4</v>
+      </c>
+      <c r="E16" s="30">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="F16" s="30">
+        <v>0.92307692299999999</v>
+      </c>
+      <c r="G16" s="30">
+        <v>1.6662498189999999</v>
+      </c>
+      <c r="H16" s="30">
+        <v>2.1339375660000002</v>
+      </c>
+      <c r="I16" s="30">
+        <v>0</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="60">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17" s="27">
+        <v>2</v>
+      </c>
+      <c r="C17" s="28">
+        <v>3</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="30">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="F17" s="30">
+        <v>0.76923076899999998</v>
+      </c>
+      <c r="G17" s="30">
+        <v>2.2784054899999999</v>
+      </c>
+      <c r="H17" s="30">
+        <v>2.2577560640000001</v>
+      </c>
+      <c r="I17" s="30">
+        <v>0</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30">
+      <c r="A18" s="24">
+        <v>18</v>
+      </c>
+      <c r="B18" s="27">
+        <v>2</v>
+      </c>
+      <c r="C18" s="28">
+        <v>4</v>
+      </c>
+      <c r="D18" s="29">
+        <v>4</v>
+      </c>
+      <c r="E18" s="30">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="F18" s="30">
+        <v>0.76923076899999998</v>
+      </c>
+      <c r="G18" s="30">
+        <v>1.8844664630000001</v>
+      </c>
+      <c r="H18" s="30">
+        <v>1.8262452579999999</v>
+      </c>
+      <c r="I18" s="30">
+        <v>0</v>
+      </c>
+      <c r="J18" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45">
+      <c r="A19" s="24">
+        <v>20</v>
+      </c>
+      <c r="B19" s="27">
+        <v>1</v>
+      </c>
+      <c r="C19" s="28">
+        <v>8</v>
+      </c>
+      <c r="D19" s="29">
+        <v>4</v>
+      </c>
+      <c r="E19" s="30">
+        <v>0.872</v>
+      </c>
+      <c r="F19" s="30">
+        <v>0.84615384599999999</v>
+      </c>
+      <c r="G19" s="30">
+        <v>2.1765301720000001</v>
+      </c>
+      <c r="H19" s="30">
+        <v>2.1339375660000002</v>
+      </c>
+      <c r="I19" s="30">
+        <v>0</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30">
+      <c r="A20" s="24">
+        <v>22</v>
+      </c>
+      <c r="B20" s="27">
+        <v>0</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="29">
+        <v>4</v>
+      </c>
+      <c r="E20" s="30">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="F20" s="30">
+        <v>0.92307692299999999</v>
+      </c>
+      <c r="G20" s="30">
+        <v>1.8488140909999999</v>
+      </c>
+      <c r="H20" s="30">
+        <v>2.0758692970000001</v>
+      </c>
+      <c r="I20" s="30">
+        <v>0</v>
+      </c>
+      <c r="J20" s="31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="24">
+        <v>22</v>
+      </c>
+      <c r="B21" s="32">
+        <v>1</v>
+      </c>
+      <c r="C21" s="33">
+        <v>8</v>
+      </c>
+      <c r="D21" s="34">
+        <v>4</v>
+      </c>
+      <c r="E21" s="35">
+        <v>0.872</v>
+      </c>
+      <c r="F21" s="35">
+        <v>0.84615384599999999</v>
+      </c>
+      <c r="G21" s="35">
+        <v>2.111059843</v>
+      </c>
+      <c r="H21" s="35">
+        <v>2.1339375660000002</v>
+      </c>
+      <c r="I21" s="35">
+        <v>0</v>
+      </c>
+      <c r="J21" s="36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30">
+      <c r="A22" s="24">
+        <v>24</v>
+      </c>
+      <c r="B22" s="27">
+        <v>4</v>
+      </c>
+      <c r="C22" s="28">
+        <v>5</v>
+      </c>
+      <c r="D22" s="29">
+        <v>4</v>
+      </c>
+      <c r="E22" s="30">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="F22" s="30">
+        <v>0.61538461499999997</v>
+      </c>
+      <c r="G22" s="30">
+        <v>1.9071985739999999</v>
+      </c>
+      <c r="H22" s="30">
+        <v>1.9220231430000001</v>
+      </c>
+      <c r="I22" s="30">
+        <v>0</v>
+      </c>
+      <c r="J22" s="31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30">
+      <c r="A23" s="24">
+        <v>36</v>
+      </c>
+      <c r="B23" s="27">
+        <v>3</v>
+      </c>
+      <c r="C23" s="28">
+        <v>3</v>
+      </c>
+      <c r="D23" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="30">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="F23" s="30">
+        <v>0.69230769199999997</v>
+      </c>
+      <c r="G23" s="30">
+        <v>2.1098479999999999</v>
+      </c>
+      <c r="H23" s="30">
+        <v>2.199687795</v>
+      </c>
+      <c r="I23" s="30">
+        <v>0</v>
+      </c>
+      <c r="J23" s="31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="24">
+        <v>36</v>
+      </c>
+      <c r="B24" s="27">
+        <v>5</v>
+      </c>
+      <c r="C24" s="28">
+        <v>12</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="30">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="F24" s="30">
+        <v>0.53846153799999996</v>
+      </c>
+      <c r="G24" s="30">
+        <v>1.9904614819999999</v>
+      </c>
+      <c r="H24" s="30">
+        <v>1.9877733710000001</v>
+      </c>
+      <c r="I24" s="30">
+        <v>0</v>
+      </c>
+      <c r="J24" s="31" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30">
+      <c r="A25" s="24">
+        <v>38</v>
+      </c>
+      <c r="B25" s="27">
+        <v>2</v>
+      </c>
+      <c r="C25" s="28">
+        <v>6</v>
+      </c>
+      <c r="D25" s="29">
+        <v>4</v>
+      </c>
+      <c r="E25" s="30">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="F25" s="30">
+        <v>0.76923076899999998</v>
+      </c>
+      <c r="G25" s="30">
+        <v>1.86212982</v>
+      </c>
+      <c r="H25" s="30">
+        <v>1.8262452579999999</v>
+      </c>
+      <c r="I25" s="30">
+        <v>0</v>
+      </c>
+      <c r="J25" s="31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="24">
+        <v>38</v>
+      </c>
+      <c r="B26" s="32">
+        <v>3</v>
+      </c>
+      <c r="C26" s="33">
+        <v>12</v>
+      </c>
+      <c r="D26" s="34">
+        <v>4</v>
+      </c>
+      <c r="E26" s="35">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="F26" s="35">
+        <v>0.69230769199999997</v>
+      </c>
+      <c r="G26" s="35">
+        <v>1.8718392930000001</v>
+      </c>
+      <c r="H26" s="35">
+        <v>1.8542858719999999</v>
+      </c>
+      <c r="I26" s="35">
+        <v>0</v>
+      </c>
+      <c r="J26" s="36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>